<commit_message>
Añadido cambios al prseupuesto debido a los riesgos
</commit_message>
<xml_diff>
--- a/P5/EstimacionesPresupuestoI+D.xlsx
+++ b/P5/EstimacionesPresupuestoI+D.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\PGPIProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\PGPIProject\P5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76842CE7-1402-49D3-BFF8-8BDC342908BB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404B15ED-41C5-4AAB-8E12-E733BEA840A1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28785" windowHeight="15495" activeTab="2" xr2:uid="{DF85E423-6D6D-425A-8C7C-A6D919EDE1EC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28785" windowHeight="15495" activeTab="1" xr2:uid="{DF85E423-6D6D-425A-8C7C-A6D919EDE1EC}"/>
   </bookViews>
   <sheets>
     <sheet name="I+d" sheetId="1" r:id="rId1"/>
-    <sheet name="Flujo de Cajas + VAN + TIR" sheetId="3" r:id="rId2"/>
-    <sheet name="Hoja1" sheetId="4" r:id="rId3"/>
+    <sheet name="i+d+risks" sheetId="5" r:id="rId2"/>
+    <sheet name="Flujo de Cajas + VAN + TIR" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="108">
   <si>
     <t>GASTOS DE PERSONAL</t>
   </si>
@@ -327,6 +328,36 @@
   </si>
   <si>
     <t>Consultoria legal</t>
+  </si>
+  <si>
+    <t>Total Sin Riesgos</t>
+  </si>
+  <si>
+    <t>Riesgos de desarrollo</t>
+  </si>
+  <si>
+    <t>Riegos de fase final</t>
+  </si>
+  <si>
+    <t>Riegos Globales</t>
+  </si>
+  <si>
+    <t>Pero Caso</t>
+  </si>
+  <si>
+    <t>Mejor Caso</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Costes adicionales (Peor Caso)</t>
+  </si>
+  <si>
+    <t>Total Con Peor Caso</t>
+  </si>
+  <si>
+    <t>Total Con Mejor Caso</t>
   </si>
 </sst>
 </file>
@@ -481,7 +512,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3"/>
@@ -493,6 +524,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="6"/>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="7"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -1706,8 +1738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E779E267-DA2E-48FF-ABF8-195CAC91C758}">
   <dimension ref="A2:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2157,6 +2189,533 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3AB4A9C-CDC2-482B-B9D3-A3B893244162}">
+  <dimension ref="A2:M40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14:J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="84.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="12" max="13" width="28.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="4">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="4">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <f>SUM(D5:D8)</f>
+        <v>70604.205000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <f>3*(2800*(1+B6))</f>
+        <v>11701.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6">
+        <f>5*(3050*(1+B6))</f>
+        <v>21243.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="4">
+        <v>23.6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7">
+        <f>5*(2887*(1+B6))</f>
+        <v>20107.954999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
+        <v>4.7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8">
+        <f>3*(4200*(1+B6))</f>
+        <v>17551.800000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2">
+        <f>SUM(D10:D27)</f>
+        <v>18553.746666666666</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11">
+        <f>((395.1+200)*(B2-2)/2)</f>
+        <v>5951</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="7">
+        <v>6.7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <f>(260 * (B2-2)/2)</f>
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="7">
+        <v>1.6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <f>4 * 156.84</f>
+        <v>627.36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14">
+        <f>B3*979</f>
+        <v>5874</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J14" s="2">
+        <f>D39*1.21</f>
+        <v>175935.71711100001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J15" s="2">
+        <f>J14+L24</f>
+        <v>524305.96578856674</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16">
+        <f>-((((D12*0.1)/20)/12)*B4)</f>
+        <v>-8.6666666666666661</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J16" s="2">
+        <f>J14+M24</f>
+        <v>300858.84065870335</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17">
+        <f>-((((D11*0.2)/10)/12)*B4)</f>
+        <v>-79.346666666666678</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19">
+        <f>11.5 * (B2/2)</f>
+        <v>126.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20">
+        <f>(17.95*(B2-2))</f>
+        <v>359</v>
+      </c>
+      <c r="I20" s="10"/>
+      <c r="J20" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21">
+        <f>((0.39*4)*8)+((1.99+4)*8)</f>
+        <v>60.400000000000006</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J21" s="2">
+        <v>30</v>
+      </c>
+      <c r="K21" s="2">
+        <v>15</v>
+      </c>
+      <c r="L21" s="2">
+        <f>SUM(D6:D7)*(J21/100)</f>
+        <v>12405.361500000001</v>
+      </c>
+      <c r="M21" s="2">
+        <f>SUM(D6:D7)*(K21/100)</f>
+        <v>6202.6807500000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22">
+        <f>170*B4</f>
+        <v>1360</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J22" s="2">
+        <v>10</v>
+      </c>
+      <c r="K22" s="2">
+        <v>5</v>
+      </c>
+      <c r="L22" s="2">
+        <f>SUM(D11:D17,D19:D22)*(J22/100)</f>
+        <v>1687.0246666666667</v>
+      </c>
+      <c r="M22" s="2">
+        <f>SUM(D11:D17,D19:D22)*(K22/100)</f>
+        <v>843.51233333333334</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="I23" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J23" s="2">
+        <v>190</v>
+      </c>
+      <c r="K23" s="2">
+        <v>67</v>
+      </c>
+      <c r="L23" s="2">
+        <f>J14*(J23/100)</f>
+        <v>334277.86251090001</v>
+      </c>
+      <c r="M23" s="2">
+        <f>J14*(K23/100)</f>
+        <v>117876.93046437002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24">
+        <v>500</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="J24" s="2">
+        <v>230</v>
+      </c>
+      <c r="K24" s="2">
+        <v>87</v>
+      </c>
+      <c r="L24" s="2">
+        <f>SUM(L21:L23)</f>
+        <v>348370.24867756671</v>
+      </c>
+      <c r="M24" s="2">
+        <f>SUM(M21:M23)</f>
+        <v>124923.12354770335</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25">
+        <v>20</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="5"/>
+    </row>
+    <row r="26" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27">
+        <f>2*(9.67*25)</f>
+        <v>483.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="2">
+        <f>SUM(D29:D37)</f>
+        <v>26240</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30">
+        <f>(50*12)*B3</f>
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31">
+        <f>(5*20*4)</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32">
+        <f>40*6</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="3:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="5"/>
+    </row>
+    <row r="36" spans="3:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="2">
+        <f>$D$28+$D$9+$D$4</f>
+        <v>115397.95166666666</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C39" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D39" s="2">
+        <f>($D$28+$D$9+$D$4)*1.26</f>
+        <v>145401.4191</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C40" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" s="2">
+        <f>D39*1.21</f>
+        <v>175935.71711100001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5802B4F9-1648-42BA-97DD-2A831C3008FA}">
   <dimension ref="A1:J38"/>
   <sheetViews>
@@ -2673,11 +3232,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC54B44-A867-4ADA-A882-2969CB1D7E7B}">
   <dimension ref="E4:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Arreglo de fallo encontrado en estimacion presupuesto y empiece de practica 8
</commit_message>
<xml_diff>
--- a/P5/EstimacionesPresupuestoI+D.xlsx
+++ b/P5/EstimacionesPresupuestoI+D.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\PGPIProject\P5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\takit\PGPIProject\P5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404B15ED-41C5-4AAB-8E12-E733BEA840A1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FB93C8-FA86-4C53-84CE-DA3334E5C617}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28785" windowHeight="15495" activeTab="1" xr2:uid="{DF85E423-6D6D-425A-8C7C-A6D919EDE1EC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{DF85E423-6D6D-425A-8C7C-A6D919EDE1EC}"/>
   </bookViews>
   <sheets>
     <sheet name="I+d" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="109">
   <si>
     <t>GASTOS DE PERSONAL</t>
   </si>
@@ -358,6 +358,9 @@
   </si>
   <si>
     <t>Total Con Mejor Caso</t>
+  </si>
+  <si>
+    <t>Total gastos de contratación de ejecutivos</t>
   </si>
 </sst>
 </file>
@@ -652,28 +655,28 @@
                   <c:v>-27164.260000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-14869.525625</c:v>
+                  <c:v>-61842.216950000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-8995.5256250000002</c:v>
+                  <c:v>-55968.216950000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-8995.5256250000002</c:v>
+                  <c:v>-55968.216950000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>61004.474374999998</c:v>
+                  <c:v>271654.63746539503</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-18995.525625000002</c:v>
+                  <c:v>-65968.216950000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-8995.5256250000002</c:v>
+                  <c:v>-55968.216950000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-8995.5256250000002</c:v>
+                  <c:v>-55968.216950000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80608.987708333341</c:v>
+                  <c:v>364865.68063169834</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1738,8 +1741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E779E267-DA2E-48FF-ABF8-195CAC91C758}">
   <dimension ref="A2:E40"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1787,7 +1790,7 @@
       </c>
       <c r="D4" s="2">
         <f>SUM(D5:D8)</f>
-        <v>70604.205000000002</v>
+        <v>287653.10700000002</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1795,7 +1798,7 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <f>3*(2800*(1+B6))</f>
+        <f>(3*(2800*(1+B6)))*1</f>
         <v>11701.2</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -1813,8 +1816,8 @@
         <v>35</v>
       </c>
       <c r="D6">
-        <f>5*(3050*(1+B6))</f>
-        <v>21243.25</v>
+        <f>(5*(3050*(1+B6)))*5.4</f>
+        <v>114713.55</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>38</v>
@@ -1831,8 +1834,8 @@
         <v>36</v>
       </c>
       <c r="D7">
-        <f>5*(2887*(1+B6))</f>
-        <v>20107.954999999998</v>
+        <f>(5*(2887*(1+B6)))*5.4</f>
+        <v>108582.95699999999</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>39</v>
@@ -1846,8 +1849,8 @@
         <v>37</v>
       </c>
       <c r="D8">
-        <f>3*(4200*(1+B6))</f>
-        <v>17551.800000000003</v>
+        <f>(3*(4200*(1+B6))*3)</f>
+        <v>52655.400000000009</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>40</v>
@@ -2153,7 +2156,7 @@
       </c>
       <c r="D38" s="2">
         <f>$D$28+$D$9+$D$4</f>
-        <v>115397.95166666666</v>
+        <v>332446.85366666666</v>
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.25">
@@ -2162,7 +2165,7 @@
       </c>
       <c r="D39" s="2">
         <f>($D$28+$D$9+$D$4)*1.26</f>
-        <v>145401.4191</v>
+        <v>418883.03561999998</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.25">
@@ -2171,7 +2174,7 @@
       </c>
       <c r="D40" s="2">
         <f>D39*1.21</f>
-        <v>175935.71711100001</v>
+        <v>506848.47310019995</v>
       </c>
     </row>
   </sheetData>
@@ -2190,10 +2193,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3AB4A9C-CDC2-482B-B9D3-A3B893244162}">
-  <dimension ref="A2:M40"/>
+  <dimension ref="A2:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14:J16"/>
+    <sheetView tabSelected="1" topLeftCell="F14" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2241,473 +2244,484 @@
         <v>0</v>
       </c>
       <c r="D4" s="2">
-        <f>SUM(D5:D8)</f>
-        <v>70604.205000000002</v>
+        <f>SUM(D5:D9)</f>
+        <v>446385.73560000001</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="4"/>
       <c r="C5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5">
+        <f>(4*(2800*(1+B7)))*5</f>
+        <v>78008</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>1</v>
       </c>
-      <c r="D5">
-        <f>3*(2800*(1+B6))</f>
-        <v>11701.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0.39300000000000002</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
       <c r="D6">
-        <f>5*(3050*(1+B6))</f>
-        <v>21243.25</v>
+        <f>4*(2800*(1+B7))</f>
+        <v>15601.6</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7">
+        <f>(7*(3050*(1+B7)))*5.4</f>
+        <v>160598.97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B8" s="4">
         <v>23.6</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>36</v>
       </c>
-      <c r="D7">
-        <f>5*(2887*(1+B6))</f>
-        <v>20107.954999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="4">
+      <c r="D8">
+        <f>(4*(2887*(1+B7)))*5.4</f>
+        <v>86866.365600000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
         <v>4.7</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>37</v>
       </c>
-      <c r="D8">
-        <f>3*(4200*(1+B6))</f>
-        <v>17551.800000000003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="D9">
+        <f>(6*(4200*(1+B7)))*3</f>
+        <v>105310.80000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B10" s="4">
         <v>0.12</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="2">
-        <f>SUM(D10:D27)</f>
+      <c r="D10" s="2">
+        <f>SUM(D11:D28)</f>
         <v>18553.746666666666</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B11" s="4">
         <v>0.6</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="7">
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="7">
         <v>0.1</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>17</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <f>((395.1+200)*(B2-2)/2)</f>
         <v>5951</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B13" s="7">
         <v>6.7</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>18</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <f>(260 * (B2-2)/2)</f>
         <v>2600</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="7">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="7">
         <v>1.6</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>19</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <f>4 * 156.84</f>
         <v>627.36</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>32</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <f>B3*979</f>
         <v>5874</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="J14" s="2">
-        <f>D39*1.21</f>
-        <v>175935.71711100001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="J15" s="2">
-        <f>J14+L24</f>
-        <v>524305.96578856674</v>
+        <f>D40*1.21</f>
+        <v>748852.23866376001</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J16" s="2">
+        <f>J15+L25</f>
+        <v>2247598.1174715706</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
         <v>52</v>
       </c>
-      <c r="D16">
-        <f>-((((D12*0.1)/20)/12)*B4)</f>
+      <c r="D17">
+        <f>-((((D13*0.1)/20)/12)*B4)</f>
         <v>-8.6666666666666661</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="J16" s="2">
-        <f>J14+M24</f>
-        <v>300858.84065870335</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
+      <c r="J17" s="2">
+        <f>J15+M25</f>
+        <v>1288546.5512418125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
         <v>53</v>
       </c>
-      <c r="D17">
-        <f>-((((D11*0.2)/10)/12)*B4)</f>
+      <c r="D18">
+        <f>-((((D12*0.2)/10)/12)*B4)</f>
         <v>-79.346666666666678</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="5" t="s">
+    <row r="19" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
         <v>30</v>
       </c>
-      <c r="D19">
+      <c r="D20">
         <f>11.5 * (B2/2)</f>
         <v>126.5</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>47</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>29</v>
       </c>
-      <c r="D20">
+      <c r="D21">
         <f>(17.95*(B2-2))</f>
         <v>359</v>
       </c>
-      <c r="I20" s="10"/>
-      <c r="J20" s="1" t="s">
+      <c r="I21" s="10"/>
+      <c r="J21" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="L21" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="M21" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>49</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>90</v>
       </c>
-      <c r="D21">
+      <c r="D22">
         <f>((0.39*4)*8)+((1.99+4)*8)</f>
         <v>60.400000000000006</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J22" s="2">
         <v>30</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K22" s="2">
         <v>15</v>
       </c>
-      <c r="L21" s="2">
-        <f>SUM(D6:D7)*(J21/100)</f>
-        <v>12405.361500000001</v>
-      </c>
-      <c r="M21" s="2">
-        <f>SUM(D6:D7)*(K21/100)</f>
-        <v>6202.6807500000004</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
+      <c r="L22" s="2">
+        <f>SUM(D7:D8)*(J22/100)</f>
+        <v>74239.600679999989</v>
+      </c>
+      <c r="M22" s="2">
+        <f>SUM(D7:D8)*(K22/100)</f>
+        <v>37119.800339999994</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
         <v>94</v>
       </c>
-      <c r="D22">
+      <c r="D23">
         <f>170*B4</f>
         <v>1360</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J23" s="2">
         <v>10</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K23" s="2">
         <v>5</v>
       </c>
-      <c r="L22" s="2">
-        <f>SUM(D11:D17,D19:D22)*(J22/100)</f>
+      <c r="L23" s="2">
+        <f>SUM(D12:D18,D20:D23)*(J23/100)</f>
         <v>1687.0246666666667</v>
       </c>
-      <c r="M22" s="2">
-        <f>SUM(D11:D17,D19:D22)*(K22/100)</f>
+      <c r="M23" s="2">
+        <f>SUM(D12:D18,D20:D23)*(K23/100)</f>
         <v>843.51233333333334</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="5" t="s">
+    <row r="24" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="5"/>
-      <c r="I23" s="1" t="s">
+      <c r="D24" s="5"/>
+      <c r="I24" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J24" s="2">
         <v>190</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K24" s="2">
         <v>67</v>
       </c>
-      <c r="L23" s="2">
-        <f>J14*(J23/100)</f>
-        <v>334277.86251090001</v>
-      </c>
-      <c r="M23" s="2">
-        <f>J14*(K23/100)</f>
-        <v>117876.93046437002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" t="s">
+      <c r="L24" s="2">
+        <f>J15*(J24/100)</f>
+        <v>1422819.2534611439</v>
+      </c>
+      <c r="M24" s="2">
+        <f>J15*(K24/100)</f>
+        <v>501730.99990471924</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
         <v>28</v>
       </c>
-      <c r="D24">
+      <c r="D25">
         <v>500</v>
       </c>
-      <c r="I24" s="11" t="s">
+      <c r="I25" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="J24" s="2">
+      <c r="J25" s="2">
         <v>230</v>
       </c>
-      <c r="K24" s="2">
+      <c r="K25" s="2">
         <v>87</v>
       </c>
-      <c r="L24" s="2">
-        <f>SUM(L21:L23)</f>
-        <v>348370.24867756671</v>
-      </c>
-      <c r="M24" s="2">
-        <f>SUM(M21:M23)</f>
-        <v>124923.12354770335</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="L25" s="2">
+        <f>SUM(L22:L24)</f>
+        <v>1498745.8788078106</v>
+      </c>
+      <c r="M25" s="2">
+        <f>SUM(M22:M24)</f>
+        <v>539694.31257805252</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>20</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="5"/>
-    </row>
-    <row r="26" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B26">
+      <c r="B27">
         <v>10</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>31</v>
       </c>
-      <c r="D26">
+      <c r="D27">
         <v>700</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
         <v>21</v>
       </c>
-      <c r="D27">
+      <c r="D28">
         <f>2*(9.67*25)</f>
         <v>483.5</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="1" t="s">
+    <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="2">
-        <f>SUM(D29:D37)</f>
+      <c r="D29" s="2">
+        <f>SUM(D30:D38)</f>
         <v>26240</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="5" t="s">
+    <row r="30" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="5"/>
-    </row>
-    <row r="30" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
         <v>22</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <f>(50*12)*B3</f>
         <v>3600</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
         <v>23</v>
       </c>
-      <c r="D31">
+      <c r="D32">
         <f>(5*20*4)</f>
         <v>400</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" t="s">
+    <row r="33" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
         <v>24</v>
       </c>
-      <c r="D32">
+      <c r="D33">
         <f>40*6</f>
         <v>240</v>
       </c>
     </row>
-    <row r="33" spans="3:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="5" t="s">
+    <row r="34" spans="3:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="5"/>
-    </row>
-    <row r="34" spans="3:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C34" t="s">
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="3:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
         <v>26</v>
       </c>
-      <c r="D34">
+      <c r="D35">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="3:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="5" t="s">
+    <row r="36" spans="3:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D35" s="5"/>
-    </row>
-    <row r="36" spans="3:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+      <c r="D36" s="5"/>
+    </row>
+    <row r="37" spans="3:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
         <v>96</v>
       </c>
-      <c r="D36">
+      <c r="D37">
         <v>22000</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
         <v>12</v>
       </c>
-      <c r="D37">
+      <c r="D38">
         <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C38" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="2">
-        <f>$D$28+$D$9+$D$4</f>
-        <v>115397.95166666666</v>
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C39" s="1" t="s">
-        <v>71</v>
+        <v>6</v>
       </c>
       <c r="D39" s="2">
-        <f>($D$28+$D$9+$D$4)*1.26</f>
-        <v>145401.4191</v>
+        <f>$D$29+$D$10+$D$4</f>
+        <v>491179.48226666666</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C40" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D40" s="2">
+        <f>($D$29+$D$10+$D$4)*1.26</f>
+        <v>618886.14765599999</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C41" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D40" s="2">
-        <f>D39*1.21</f>
-        <v>175935.71711100001</v>
+      <c r="D41" s="2">
+        <f>D40*1.21</f>
+        <v>748852.23866376001</v>
       </c>
     </row>
   </sheetData>
@@ -2720,7 +2734,7 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2764,10 +2778,12 @@
         <v>57</v>
       </c>
       <c r="F2">
-        <v>70000</v>
+        <f>B18*0.4375</f>
+        <v>327622.85441539501</v>
       </c>
       <c r="J2">
-        <v>90000</v>
+        <f>B18*0.5625</f>
+        <v>421229.38424836501</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2806,35 +2822,35 @@
       </c>
       <c r="C6">
         <f>-(B23/8)</f>
-        <v>-8825.5256250000002</v>
+        <v>-55798.216950000002</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D6:J6" si="0">-8825.525625</f>
-        <v>-8825.5256250000002</v>
+        <f>$C$6</f>
+        <v>-55798.216950000002</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
-        <v>-8825.5256250000002</v>
+        <f t="shared" ref="E6:J6" si="0">$C$6</f>
+        <v>-55798.216950000002</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>-8825.5256250000002</v>
+        <v>-55798.216950000002</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>-8825.5256250000002</v>
+        <v>-55798.216950000002</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>-8825.5256250000002</v>
+        <v>-55798.216950000002</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>-8825.5256250000002</v>
+        <v>-55798.216950000002</v>
       </c>
       <c r="J6">
         <f t="shared" si="0"/>
-        <v>-8825.5256250000002</v>
+        <v>-55798.216950000002</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2956,7 +2972,7 @@
         <v>69</v>
       </c>
       <c r="B18" s="4">
-        <v>175935.71711100001</v>
+        <v>748852.23866376001</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -2965,7 +2981,7 @@
       </c>
       <c r="B19" s="4">
         <f>-(SUM(B3:J16))</f>
-        <v>115397.95166666665</v>
+        <v>491179.48226666683</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -2974,7 +2990,7 @@
       </c>
       <c r="B20" s="4">
         <f>B18-B19</f>
-        <v>60537.765444333359</v>
+        <v>257672.75639709318</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2983,7 +2999,7 @@
       </c>
       <c r="B21">
         <f>B20*0.21</f>
-        <v>12712.930743310006</v>
+        <v>54111.278843389569</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -3000,7 +3016,7 @@
         <v>74</v>
       </c>
       <c r="B23">
-        <v>70604.205000000002</v>
+        <v>446385.73560000001</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3014,35 +3030,35 @@
       </c>
       <c r="C26">
         <f t="shared" si="2"/>
-        <v>-14869.525625</v>
+        <v>-61842.216950000002</v>
       </c>
       <c r="D26">
         <f t="shared" si="2"/>
-        <v>-8995.5256250000002</v>
+        <v>-55968.216950000002</v>
       </c>
       <c r="E26">
         <f t="shared" si="2"/>
-        <v>-8995.5256250000002</v>
+        <v>-55968.216950000002</v>
       </c>
       <c r="F26">
         <f t="shared" si="2"/>
-        <v>61004.474374999998</v>
+        <v>271654.63746539503</v>
       </c>
       <c r="G26">
         <f t="shared" si="2"/>
-        <v>-18995.525625000002</v>
+        <v>-65968.216950000002</v>
       </c>
       <c r="H26">
         <f t="shared" si="2"/>
-        <v>-8995.5256250000002</v>
+        <v>-55968.216950000002</v>
       </c>
       <c r="I26">
         <f t="shared" si="2"/>
-        <v>-8995.5256250000002</v>
+        <v>-55968.216950000002</v>
       </c>
       <c r="J26">
         <f t="shared" si="2"/>
-        <v>80608.987708333341</v>
+        <v>364865.68063169834</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3055,35 +3071,35 @@
       </c>
       <c r="C27">
         <f>SUM(B26:C26)</f>
-        <v>-42033.785625000004</v>
+        <v>-89006.476950000011</v>
       </c>
       <c r="D27">
         <f>SUM(B26:D26)</f>
-        <v>-51029.311250000006</v>
+        <v>-144974.69390000001</v>
       </c>
       <c r="E27">
         <f>SUM(B26:E26)</f>
-        <v>-60024.836875000008</v>
+        <v>-200942.91085000001</v>
       </c>
       <c r="F27">
         <f>SUM(B26:F26)</f>
-        <v>979.63749999998981</v>
+        <v>70711.726615395019</v>
       </c>
       <c r="G27">
         <f>SUM(B26:G26)</f>
-        <v>-18015.888125000012</v>
+        <v>4743.5096653950168</v>
       </c>
       <c r="H27">
         <f>SUM(B26:H26)</f>
-        <v>-27011.413750000014</v>
+        <v>-51224.707284604985</v>
       </c>
       <c r="I27">
         <f>SUM(B26:I26)</f>
-        <v>-36006.939375000016</v>
+        <v>-107192.92423460499</v>
       </c>
       <c r="J27">
         <f>SUM(B26:J26)</f>
-        <v>44602.048333333325</v>
+        <v>257672.75639709336</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3130,11 +3146,11 @@
       </c>
       <c r="F30">
         <f>F27/(1+B28)</f>
-        <v>882.55630630629707</v>
+        <v>63704.25821206758</v>
       </c>
       <c r="J30">
         <f>J27/POWER((1+B28), 2)</f>
-        <v>36200.022995968931</v>
+        <v>209132.98952771147</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -3143,7 +3159,7 @@
       </c>
       <c r="B31" s="4">
         <f>SUM(B30:J30)</f>
-        <v>9918.3193022752275</v>
+        <v>245672.98773977906</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3190,19 +3206,19 @@
       </c>
       <c r="D35">
         <f>D27/POWER(1+B33,2)</f>
-        <v>-47179.466762204145</v>
+        <v>-134037.25397559171</v>
       </c>
       <c r="F35">
         <f>F27/POWER(1+B33,3)</f>
-        <v>870.89417031746927</v>
+        <v>62862.467476419384</v>
       </c>
       <c r="H35">
         <f>F27/POWER(1+B33,4)</f>
-        <v>837.39824068987423</v>
+        <v>60444.680265787865</v>
       </c>
       <c r="J35">
         <f>J27/POWER((1+B33), 5)</f>
-        <v>36659.632542157415</v>
+        <v>211788.22315617013</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -3211,7 +3227,7 @@
       </c>
       <c r="B36" s="8">
         <f>SUM(B35:J35)</f>
-        <v>-35975.801809039389</v>
+        <v>173893.85692278566</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>87</v>
@@ -3223,7 +3239,7 @@
       </c>
       <c r="B38" s="9">
         <f>IRR(B26:J26)</f>
-        <v>0.11124775350786575</v>
+        <v>0.21007509138405411</v>
       </c>
     </row>
   </sheetData>

</xml_diff>